<commit_message>
Updates to bldgs/BDEQ, bldgs/SYDEC and the calibration sheet - updated with Canada specific residential ratios from bldgs/BCEU
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SYDEC/Start Year Distributed Electricity Capacity.xlsx
+++ b/InputData/bldgs/SYDEC/Start Year Distributed Electricity Capacity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shelley\Dropbox (Energy Innovation)\PC (2)\Documents\GitHub_Repositories\eps-canada\InputData\bldgs\SYDEC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98C722E-D33D-402D-98AA-594B2C964775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE54983F-47B6-4EB2-87CE-26520540F6F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15345" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{EAFC2935-000E-413A-B5D2-814429F7674A}"/>
+    <workbookView xWindow="-13455" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{EAFC2935-000E-413A-B5D2-814429F7674A}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="20" r:id="rId1"/>
@@ -992,10 +992,6 @@
 </externalLink>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1447,7 +1443,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1495,7 +1491,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="10">
-        <v>60.027374635579548</v>
+        <v>51.268617947930522</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -1523,7 +1519,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="10">
-        <v>54.406187677896298</v>
+        <v>46.467633592094053</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -1531,13 +1527,13 @@
         <v>10</v>
       </c>
       <c r="B6" s="10">
-        <v>0.47358467243793312</v>
+        <v>0.26888826085434137</v>
       </c>
       <c r="C6" s="10">
-        <v>0.10887166553755355</v>
+        <v>0.39610850719915114</v>
       </c>
       <c r="D6" s="10">
-        <v>144.87100001343023</v>
+        <v>123.7324803310796</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -1545,13 +1541,13 @@
         <v>11</v>
       </c>
       <c r="B7" s="10">
-        <v>609.55741389656475</v>
+        <v>346.08981762389692</v>
       </c>
       <c r="C7" s="10">
-        <v>140.13023383982159</v>
+        <v>509.83676483403775</v>
       </c>
       <c r="D7" s="10">
-        <v>442.59342907199169</v>
+        <v>378.01342402715841</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -1579,7 +1575,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="10">
-        <v>22.601285673472983</v>
+        <v>19.303470914060487</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -1607,7 +1603,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="10">
-        <v>4.1656748532671442</v>
+        <v>3.5578499616884471</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -1701,35 +1697,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <of2ed5e60f3c4f8984f283882cb94320 xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </of2ed5e60f3c4f8984f283882cb94320>
-    <ff7c4ad8664a4671b57370e258acad6a xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ff7c4ad8664a4671b57370e258acad6a>
-    <l787e5950a9249679d0130235a9a791b xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l787e5950a9249679d0130235a9a791b>
-    <TaxCatchAll xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="de340059-046a-4f1a-8b62-ade039df3700">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010010EB76B7FE121F489C7B2A4727FCE3E9" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fdee17017a9ad5b872047a216f95da93">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="52604411-7aeb-406e-8b34-4ce79a7293cc" xmlns:ns3="de340059-046a-4f1a-8b62-ade039df3700" xmlns:ns4="d580559a-617d-4d7d-8fb9-71ff64b58360" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="37825e9edfcb807d863c63152c6d8635" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="52604411-7aeb-406e-8b34-4ce79a7293cc"/>
@@ -1989,26 +1956,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4258C245-6F40-442D-84B2-78F120B3B613}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <of2ed5e60f3c4f8984f283882cb94320 xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </of2ed5e60f3c4f8984f283882cb94320>
+    <ff7c4ad8664a4671b57370e258acad6a xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ff7c4ad8664a4671b57370e258acad6a>
+    <l787e5950a9249679d0130235a9a791b xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l787e5950a9249679d0130235a9a791b>
+    <TaxCatchAll xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="de340059-046a-4f1a-8b62-ade039df3700">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F44BB7F-98DC-4BF7-9D42-02009DD39433}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="52604411-7aeb-406e-8b34-4ce79a7293cc"/>
-    <ds:schemaRef ds:uri="de340059-046a-4f1a-8b62-ade039df3700"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8014DE6-006A-45C6-BB90-1E73EA283889}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2026,4 +2003,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F44BB7F-98DC-4BF7-9D42-02009DD39433}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="52604411-7aeb-406e-8b34-4ce79a7293cc"/>
+    <ds:schemaRef ds:uri="de340059-046a-4f1a-8b62-ade039df3700"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4258C245-6F40-442D-84B2-78F120B3B613}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updates to bldgs/BDEQ and bldgs/SYDEC with recently updated elec capacity factors from elec/BECF
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SYDEC/Start Year Distributed Electricity Capacity.xlsx
+++ b/InputData/bldgs/SYDEC/Start Year Distributed Electricity Capacity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shelley\Dropbox (Energy Innovation)\PC (2)\Documents\GitHub_Repositories\eps-canada\InputData\bldgs\SYDEC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE54983F-47B6-4EB2-87CE-26520540F6F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F3A68C-3B45-4C24-8BFC-65446A56ABD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-13455" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{EAFC2935-000E-413A-B5D2-814429F7674A}"/>
   </bookViews>
@@ -1443,7 +1443,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1957,6 +1957,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <of2ed5e60f3c4f8984f283882cb94320 xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
@@ -1974,15 +1983,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2006,6 +2006,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4258C245-6F40-442D-84B2-78F120B3B613}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F44BB7F-98DC-4BF7-9D42-02009DD39433}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2014,12 +2022,4 @@
     <ds:schemaRef ds:uri="de340059-046a-4f1a-8b62-ade039df3700"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4258C245-6F40-442D-84B2-78F120B3B613}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>